<commit_message>
Data & AI showflow update with new unified repo link
</commit_message>
<xml_diff>
--- a/data-ai/Data-AI-Track-Showflow.xlsx
+++ b/data-ai/Data-AI-Track-Showflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Solliance-CloudCore-2020\data-ai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3B213-8489-4C84-A200-D863C689C673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D2CD1A-E013-4AD9-8FED-82FEAF5FFAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="49368" windowHeight="25536" activeTab="3" xr2:uid="{0B725299-4060-418E-A1A8-086098773DCE}"/>
+    <workbookView xWindow="-42540" yWindow="3492" windowWidth="36864" windowHeight="18684" activeTab="3" xr2:uid="{0B725299-4060-418E-A1A8-086098773DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>Segment</t>
   </si>
@@ -124,12 +124,6 @@
   </si>
   <si>
     <t>Team Challenge: Machine Learning PoC</t>
-  </si>
-  <si>
-    <t>Here's the link to the GitHub repo: https://github.com/solliancenet/cloudcore-2020-data-ai. The content for this WDS is located in Day-3/wds.</t>
-  </si>
-  <si>
-    <t>Here's the link to the GitHub repo: https://github.com/solliancenet/cloudcore-2020-data-ai. The content for this hands-on is located in Day-3/challenge.</t>
   </si>
   <si>
     <t>WDS: IoT and the Smary City as an ADS</t>
@@ -2422,7 +2416,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -2430,7 +2424,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N20" s="9"/>
     </row>
@@ -2504,7 +2498,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -2512,7 +2506,7 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N23" s="9"/>
     </row>
@@ -3309,7 +3303,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -3702,7 +3696,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -3710,7 +3704,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N20" s="9"/>
     </row>
@@ -3784,7 +3778,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -3792,7 +3786,7 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N23" s="9"/>
     </row>
@@ -4589,7 +4583,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
@@ -4952,7 +4946,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -4982,7 +4976,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -4990,7 +4984,7 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N20" s="9"/>
     </row>
@@ -5008,7 +5002,7 @@
         <v>9.0277777777777776E-2</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="25"/>
@@ -5062,7 +5056,7 @@
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -5070,9 +5064,9 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="N23" s="38"/>
     </row>
     <row r="24" spans="1:14" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
@@ -5088,7 +5082,7 @@
         <v>7.9861111111111105E-2</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -5852,7 +5846,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{6770C0F2-321E-40BB-A2A1-A54547EEC619}"/>
-    <hyperlink ref="M23" r:id="rId2" display="https://github.com/solliancenet/cloud-core-2020" xr:uid="{AFFFAC54-0DE1-4BE8-AFF7-77BD947ED736}"/>
+    <hyperlink ref="M23" r:id="rId2" xr:uid="{5DB0A3FB-7892-44D0-B506-636C6F89A187}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId3"/>

</xml_diff>